<commit_message>
Atualização Capacidade Vinculada MRS
</commit_message>
<xml_diff>
--- a/Dados/dr2020_original.xlsx
+++ b/Dados/dr2020_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020\ANTT\Interface_Graf_GitHub\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA08484-902D-4A67-92B6-F881C4A9C6B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B409CAF6-08E4-476C-8C57-4C07A5362C19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Página 1'!$A$1:$M$1865</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45649,10 +45649,10 @@
         <v>16.363636363636363</v>
       </c>
       <c r="L952" s="10">
-        <v>0</v>
+        <v>5.4153846153846157</v>
       </c>
       <c r="M952" s="10">
-        <v>0</v>
+        <v>5.046153846153846</v>
       </c>
     </row>
     <row r="953" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -46100,10 +46100,10 @@
         <v>17</v>
       </c>
       <c r="L963" s="10">
-        <v>0</v>
+        <v>6.6934911242603548</v>
       </c>
       <c r="M963" s="10">
-        <v>0</v>
+        <v>6.5230769230769239</v>
       </c>
     </row>
     <row r="964" spans="1:13" x14ac:dyDescent="0.3">
@@ -46141,10 +46141,10 @@
         <v>17</v>
       </c>
       <c r="L964" s="10">
-        <v>0</v>
+        <v>6.6934911242603548</v>
       </c>
       <c r="M964" s="10">
-        <v>0</v>
+        <v>6.5230769230769239</v>
       </c>
     </row>
     <row r="965" spans="1:13" x14ac:dyDescent="0.3">
@@ -46182,10 +46182,10 @@
         <v>17</v>
       </c>
       <c r="L965" s="10">
-        <v>0</v>
+        <v>6.6934911242603548</v>
       </c>
       <c r="M965" s="10">
-        <v>0</v>
+        <v>6.5230769230769239</v>
       </c>
     </row>
     <row r="966" spans="1:13" x14ac:dyDescent="0.3">
@@ -46223,10 +46223,10 @@
         <v>17</v>
       </c>
       <c r="L966" s="10">
-        <v>0</v>
+        <v>6.6934911242603548</v>
       </c>
       <c r="M966" s="10">
-        <v>0</v>
+        <v>6.5230769230769239</v>
       </c>
     </row>
     <row r="967" spans="1:13" x14ac:dyDescent="0.3">
@@ -46264,10 +46264,10 @@
         <v>17</v>
       </c>
       <c r="L967" s="10">
-        <v>0</v>
+        <v>6.6934911242603548</v>
       </c>
       <c r="M967" s="10">
-        <v>0</v>
+        <v>6.5230769230769239</v>
       </c>
     </row>
     <row r="968" spans="1:13" x14ac:dyDescent="0.3">
@@ -46305,10 +46305,10 @@
         <v>17</v>
       </c>
       <c r="L968" s="10">
-        <v>0</v>
+        <v>8.0227218934911253</v>
       </c>
       <c r="M968" s="10">
-        <v>0</v>
+        <v>7.4725274725274726</v>
       </c>
     </row>
     <row r="969" spans="1:13" x14ac:dyDescent="0.3">
@@ -46346,10 +46346,10 @@
         <v>25</v>
       </c>
       <c r="L969" s="10">
-        <v>0</v>
+        <v>5.7088757396449701</v>
       </c>
       <c r="M969" s="10">
-        <v>0</v>
+        <v>6.8571428571428577</v>
       </c>
     </row>
     <row r="970" spans="1:13" x14ac:dyDescent="0.3">
@@ -46387,10 +46387,10 @@
         <v>25</v>
       </c>
       <c r="L970" s="10">
-        <v>0</v>
+        <v>6.3652859960552277</v>
       </c>
       <c r="M970" s="10">
-        <v>0</v>
+        <v>7.5135531135531135</v>
       </c>
     </row>
     <row r="971" spans="1:13" x14ac:dyDescent="0.3">
@@ -46428,10 +46428,10 @@
         <v>25</v>
       </c>
       <c r="L971" s="10">
-        <v>0</v>
+        <v>6.3652859960552277</v>
       </c>
       <c r="M971" s="10">
-        <v>0</v>
+        <v>7.5135531135531135</v>
       </c>
     </row>
     <row r="972" spans="1:13" x14ac:dyDescent="0.3">
@@ -46469,10 +46469,10 @@
         <v>25</v>
       </c>
       <c r="L972" s="10">
-        <v>0</v>
+        <v>3.9794871794871796</v>
       </c>
       <c r="M972" s="10">
-        <v>0</v>
+        <v>4.9289377289377292</v>
       </c>
     </row>
     <row r="973" spans="1:13" x14ac:dyDescent="0.3">
@@ -46510,10 +46510,10 @@
         <v>25</v>
       </c>
       <c r="L973" s="10">
-        <v>0</v>
+        <v>3.9794871794871796</v>
       </c>
       <c r="M973" s="10">
-        <v>0</v>
+        <v>6.7340659340659332</v>
       </c>
     </row>
     <row r="974" spans="1:13" x14ac:dyDescent="0.3">
@@ -46551,10 +46551,10 @@
         <v>25</v>
       </c>
       <c r="L974" s="10">
-        <v>0</v>
+        <v>5.3825641025641024</v>
       </c>
       <c r="M974" s="10">
-        <v>0</v>
+        <v>6.7340659340659332</v>
       </c>
     </row>
     <row r="975" spans="1:13" x14ac:dyDescent="0.3">
@@ -46592,10 +46592,10 @@
         <v>18</v>
       </c>
       <c r="L975" s="10">
-        <v>0</v>
+        <v>5.3825641025641024</v>
       </c>
       <c r="M975" s="10">
-        <v>0</v>
+        <v>5.7846153846153845</v>
       </c>
     </row>
     <row r="976" spans="1:13" x14ac:dyDescent="0.3">
@@ -46633,10 +46633,10 @@
         <v>18</v>
       </c>
       <c r="L976" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M976" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="977" spans="1:13" x14ac:dyDescent="0.3">
@@ -46674,10 +46674,10 @@
         <v>18</v>
       </c>
       <c r="L977" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M977" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="978" spans="1:13" x14ac:dyDescent="0.3">
@@ -46715,10 +46715,10 @@
         <v>18</v>
       </c>
       <c r="L978" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M978" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="979" spans="1:13" x14ac:dyDescent="0.3">
@@ -46756,10 +46756,10 @@
         <v>18</v>
       </c>
       <c r="L979" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M979" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="980" spans="1:13" x14ac:dyDescent="0.3">
@@ -46797,10 +46797,10 @@
         <v>18</v>
       </c>
       <c r="L980" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M980" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="981" spans="1:13" x14ac:dyDescent="0.3">
@@ -46838,10 +46838,10 @@
         <v>18</v>
       </c>
       <c r="L981" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M981" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="982" spans="1:13" x14ac:dyDescent="0.3">
@@ -46879,10 +46879,10 @@
         <v>22</v>
       </c>
       <c r="L982" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M982" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="983" spans="1:13" x14ac:dyDescent="0.3">
@@ -46920,10 +46920,10 @@
         <v>22</v>
       </c>
       <c r="L983" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M983" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="984" spans="1:13" x14ac:dyDescent="0.3">
@@ -46961,10 +46961,10 @@
         <v>22</v>
       </c>
       <c r="L984" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M984" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="985" spans="1:13" x14ac:dyDescent="0.3">
@@ -47002,10 +47002,10 @@
         <v>22</v>
       </c>
       <c r="L985" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M985" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="986" spans="1:13" x14ac:dyDescent="0.3">
@@ -47043,10 +47043,10 @@
         <v>22</v>
       </c>
       <c r="L986" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M986" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="987" spans="1:13" x14ac:dyDescent="0.3">
@@ -47084,10 +47084,10 @@
         <v>22</v>
       </c>
       <c r="L987" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M987" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="988" spans="1:13" x14ac:dyDescent="0.3">
@@ -47125,10 +47125,10 @@
         <v>22</v>
       </c>
       <c r="L988" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M988" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="989" spans="1:13" x14ac:dyDescent="0.3">
@@ -47166,10 +47166,10 @@
         <v>22</v>
       </c>
       <c r="L989" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M989" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="990" spans="1:13" x14ac:dyDescent="0.3">
@@ -47207,10 +47207,10 @@
         <v>22</v>
       </c>
       <c r="L990" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M990" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="991" spans="1:13" x14ac:dyDescent="0.3">
@@ -47248,10 +47248,10 @@
         <v>22</v>
       </c>
       <c r="L991" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M991" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="992" spans="1:13" x14ac:dyDescent="0.3">
@@ -47289,10 +47289,10 @@
         <v>22</v>
       </c>
       <c r="L992" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M992" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="993" spans="1:13" x14ac:dyDescent="0.3">
@@ -47330,10 +47330,10 @@
         <v>22</v>
       </c>
       <c r="L993" s="10">
-        <v>0</v>
+        <v>3.655384615384615</v>
       </c>
       <c r="M993" s="10">
-        <v>0</v>
+        <v>3.7140271493212671</v>
       </c>
     </row>
     <row r="994" spans="1:13" x14ac:dyDescent="0.3">
@@ -47494,10 +47494,10 @@
         <v>8</v>
       </c>
       <c r="L997" s="10">
-        <v>0</v>
+        <v>2.7938461538461539</v>
       </c>
       <c r="M997" s="10">
-        <v>0</v>
+        <v>2.4504374057315235</v>
       </c>
     </row>
     <row r="998" spans="1:13" x14ac:dyDescent="0.3">
@@ -47535,10 +47535,10 @@
         <v>8</v>
       </c>
       <c r="L998" s="10">
-        <v>0</v>
+        <v>2.7938461538461539</v>
       </c>
       <c r="M998" s="10">
-        <v>0</v>
+        <v>2.4504374057315235</v>
       </c>
     </row>
     <row r="999" spans="1:13" x14ac:dyDescent="0.3">
@@ -47576,10 +47576,10 @@
         <v>8</v>
       </c>
       <c r="L999" s="10">
-        <v>0</v>
+        <v>2.7938461538461539</v>
       </c>
       <c r="M999" s="10">
-        <v>0</v>
+        <v>2.4504374057315235</v>
       </c>
     </row>
     <row r="1000" spans="1:13" x14ac:dyDescent="0.3">
@@ -47617,10 +47617,10 @@
         <v>8</v>
       </c>
       <c r="L1000" s="10">
-        <v>0</v>
+        <v>2.7938461538461539</v>
       </c>
       <c r="M1000" s="10">
-        <v>0</v>
+        <v>2.4504374057315235</v>
       </c>
     </row>
     <row r="1001" spans="1:13" x14ac:dyDescent="0.3">
@@ -47781,10 +47781,10 @@
         <v>14</v>
       </c>
       <c r="L1004" s="10">
-        <v>0</v>
+        <v>5.476923076923077</v>
       </c>
       <c r="M1004" s="10">
-        <v>0</v>
+        <v>4.430769230769231</v>
       </c>
     </row>
     <row r="1005" spans="1:13" x14ac:dyDescent="0.3">
@@ -47822,10 +47822,10 @@
         <v>14</v>
       </c>
       <c r="L1005" s="10">
-        <v>0</v>
+        <v>4.9230769230769234</v>
       </c>
       <c r="M1005" s="10">
-        <v>0</v>
+        <v>4.430769230769231</v>
       </c>
     </row>
     <row r="1006" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>